<commit_message>
combined amazon size fractions
</commit_message>
<xml_diff>
--- a/analyses/T7-incubations/unipept/GO/primary-prod/BY_pp_combined.xlsx
+++ b/analyses/T7-incubations/unipept/GO/primary-prod/BY_pp_combined.xlsx
@@ -46,7 +46,7 @@
     <t xml:space="preserve">Time 0</t>
   </si>
   <si>
-    <t xml:space="preserve">Time 24 small</t>
+    <t xml:space="preserve">Time 24 hrs</t>
   </si>
 </sst>
 </file>
@@ -120,8 +120,12 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -145,7 +149,7 @@
   <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D7" activeCellId="0" sqref="D7"/>
+      <selection pane="topLeft" activeCell="B7" activeCellId="0" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -160,7 +164,7 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
@@ -210,7 +214,7 @@
         <v>8</v>
       </c>
       <c r="B3" s="0" t="n">
-        <v>0.014707444418116</v>
+        <v>0.065740715048571</v>
       </c>
       <c r="C3" s="0" t="n">
         <v>0</v>

</xml_diff>